<commit_message>
Added serial number to identify which table needs to be inserted first
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/ExaminationModule_Schema.xlsx
+++ b/application-service/src/test/resources/document/ExaminationModule_Schema.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Munawar\Work\StudentManagementSystem\application-service\src\test\resources\document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="140" windowWidth="20120" windowHeight="7940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -303,7 +308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +384,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -483,6 +494,16 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,16 +516,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,6 +526,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -562,7 +577,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -597,7 +612,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -806,44 +821,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M47"/>
+  <dimension ref="B1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B1" s="25">
+        <v>2</v>
+      </c>
+      <c r="J1" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="J2" s="15" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="J2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -869,7 +892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" s="9">
         <v>1</v>
       </c>
@@ -895,7 +918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="9">
         <v>2</v>
       </c>
@@ -921,7 +944,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B6" s="25">
+        <v>5</v>
+      </c>
       <c r="J6" s="3">
         <v>3</v>
       </c>
@@ -932,16 +958,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B7" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
@@ -957,8 +983,11 @@
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J8" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="12">
         <v>1</v>
       </c>
@@ -974,14 +1003,14 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="23"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="12">
         <v>2</v>
       </c>
@@ -1010,7 +1039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="J11" s="4">
         <v>1</v>
       </c>
@@ -1024,7 +1053,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B12" s="25">
+        <v>7</v>
+      </c>
       <c r="J12" s="4">
         <v>2</v>
       </c>
@@ -1038,16 +1070,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B13" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
       <c r="J13" s="3">
         <v>3</v>
       </c>
@@ -1061,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
@@ -1084,7 +1116,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B15" s="14">
         <v>1</v>
       </c>
@@ -1104,8 +1136,11 @@
       <c r="H15" s="11">
         <v>43713</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J15" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16" s="14">
         <v>2</v>
       </c>
@@ -1125,14 +1160,14 @@
       <c r="H16" s="11">
         <v>43713</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="17"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="23"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
       <c r="J17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1146,15 +1181,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B18" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
       <c r="J18" s="5">
         <v>1</v>
       </c>
@@ -1168,7 +1203,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
@@ -1200,7 +1235,7 @@
         <v>44256</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B20" s="7">
         <v>1</v>
       </c>
@@ -1219,8 +1254,11 @@
       <c r="G20" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J20" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B21" s="7">
         <v>2</v>
       </c>
@@ -1239,14 +1277,14 @@
       <c r="G21" s="5">
         <v>1</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="J21" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="17"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="23"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B22" s="7">
         <v>3</v>
       </c>
@@ -1278,7 +1316,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
       <c r="J23" s="8">
         <v>1</v>
       </c>
@@ -1292,7 +1330,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
       <c r="J24" s="8">
         <v>2</v>
       </c>
@@ -1306,16 +1344,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B25" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1332,7 +1370,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B27" s="13">
         <v>1</v>
       </c>
@@ -1349,7 +1387,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>2</v>
       </c>
@@ -1366,7 +1404,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <v>3</v>
       </c>
@@ -1383,18 +1421,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B32" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>66</v>
       </c>
@@ -1417,7 +1455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" s="3">
         <v>1</v>
       </c>
@@ -1438,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" s="3">
         <v>2</v>
       </c>
@@ -1459,18 +1497,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="22" t="s">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B37" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
         <v>73</v>
       </c>
@@ -1493,7 +1536,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" s="3">
         <v>1</v>
       </c>
@@ -1506,17 +1549,17 @@
       <c r="E40" s="3">
         <v>1</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G40" s="21">
+      <c r="G40" s="17">
         <v>43525</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" s="3">
         <v>2</v>
       </c>
@@ -1529,33 +1572,36 @@
       <c r="E41" s="3">
         <v>1</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="G41" s="21">
+      <c r="G41" s="17">
         <v>43526</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" s="25">
+        <v>9</v>
+      </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>85</v>
       </c>
@@ -1568,11 +1614,11 @@
       <c r="E45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" s="3">
         <v>1</v>
       </c>
@@ -1585,11 +1631,11 @@
       <c r="E46" s="3">
         <v>1</v>
       </c>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" s="3">
         <v>2</v>
       </c>
@@ -1602,9 +1648,9 @@
       <c r="E47" s="3">
         <v>1</v>
       </c>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1632,7 +1678,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1644,7 +1690,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Employee schema excel sheet tab
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/ExaminationModule_Schema.xlsx
+++ b/application-service/src/test/resources/document/ExaminationModule_Schema.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Munawar\Work\StudentManagementSystem\application-service\src\test\resources\document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="140" windowWidth="20120" windowHeight="7940"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Employee" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="189">
   <si>
     <t>Exam</t>
   </si>
@@ -285,6 +280,309 @@
   </si>
   <si>
     <t>AudienceID</t>
+  </si>
+  <si>
+    <t>Id_Employee</t>
+  </si>
+  <si>
+    <t>Id_Qualification</t>
+  </si>
+  <si>
+    <t>ID_Area</t>
+  </si>
+  <si>
+    <t>ECode</t>
+  </si>
+  <si>
+    <t>IsMale</t>
+  </si>
+  <si>
+    <t>IsMarried</t>
+  </si>
+  <si>
+    <t>FatherOrHusband</t>
+  </si>
+  <si>
+    <t>NICNo</t>
+  </si>
+  <si>
+    <t>NICExpiredOn</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Contact1</t>
+  </si>
+  <si>
+    <t>Contact2</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>BankAccount</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>OnProbation</t>
+  </si>
+  <si>
+    <t>DOJ</t>
+  </si>
+  <si>
+    <t>DOP</t>
+  </si>
+  <si>
+    <t>IsLeft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CauseOfLeaving </t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Munawar</t>
+  </si>
+  <si>
+    <t>Saad</t>
+  </si>
+  <si>
+    <t>EC2</t>
+  </si>
+  <si>
+    <t>EC1</t>
+  </si>
+  <si>
+    <t>FatherName</t>
+  </si>
+  <si>
+    <t>NIC</t>
+  </si>
+  <si>
+    <t>EmployeeExperience</t>
+  </si>
+  <si>
+    <t>ID_EmployeeExperience</t>
+  </si>
+  <si>
+    <t>ID_Employee</t>
+  </si>
+  <si>
+    <t>WorkedAs</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Gallant School</t>
+  </si>
+  <si>
+    <t>EmployeeJob</t>
+  </si>
+  <si>
+    <t>Id_EmployeeJob</t>
+  </si>
+  <si>
+    <t>ID_Designation</t>
+  </si>
+  <si>
+    <t>ID_PayScale</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>TaxDeduction</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Id_Designation</t>
+  </si>
+  <si>
+    <t>ID_Department</t>
+  </si>
+  <si>
+    <t>ID_Parent</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Id_Department</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>is designation id</t>
+  </si>
+  <si>
+    <t>PayScale</t>
+  </si>
+  <si>
+    <t>Id_PayScale</t>
+  </si>
+  <si>
+    <t>ProbationMonths</t>
+  </si>
+  <si>
+    <t>AnnualIncrementRate</t>
+  </si>
+  <si>
+    <t>Probation</t>
+  </si>
+  <si>
+    <t>Perminanet</t>
+  </si>
+  <si>
+    <t>PayScaleSalary</t>
+  </si>
+  <si>
+    <t>Id_PayScaleSalary</t>
+  </si>
+  <si>
+    <t>Id_Account</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>ProbationAmount</t>
+  </si>
+  <si>
+    <t>IsEarning</t>
+  </si>
+  <si>
+    <t>IsMain</t>
+  </si>
+  <si>
+    <t>IsPercent</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Id_AccountSubGroup</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>IsLocked</t>
+  </si>
+  <si>
+    <t>AC1</t>
+  </si>
+  <si>
+    <t>AC2</t>
+  </si>
+  <si>
+    <t>AccountSubGroup</t>
+  </si>
+  <si>
+    <t>Id_AccountGroup</t>
+  </si>
+  <si>
+    <t>AccountGroup</t>
+  </si>
+  <si>
+    <t>Id_AccountType</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>OrderNo</t>
+  </si>
+  <si>
+    <t>EmployeeSkill</t>
+  </si>
+  <si>
+    <t>ID_EmployeeSkill</t>
+  </si>
+  <si>
+    <t>ID_Skill</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Id_Skill</t>
+  </si>
+  <si>
+    <t>Swimming</t>
+  </si>
+  <si>
+    <t>Dancing</t>
+  </si>
+  <si>
+    <t>Singing</t>
+  </si>
+  <si>
+    <t>Swim well</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>EmployeeIDCard</t>
+  </si>
+  <si>
+    <t>Id_EmployeeIDCard</t>
+  </si>
+  <si>
+    <t>IssueDate</t>
+  </si>
+  <si>
+    <t>ExpiryDate</t>
+  </si>
+  <si>
+    <t>IsExpired</t>
+  </si>
+  <si>
+    <t>EmployeeAttendance</t>
+  </si>
+  <si>
+    <t>Id_EmployeeAttendance</t>
+  </si>
+  <si>
+    <t>Id_AttendanceStatus</t>
+  </si>
+  <si>
+    <t>AttendanceStatus</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Late</t>
+  </si>
+  <si>
+    <t>EmployeeSalary</t>
+  </si>
+  <si>
+    <t>Id_EmployeeSalary</t>
   </si>
 </sst>
 </file>
@@ -308,7 +606,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +688,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -498,6 +838,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -516,7 +857,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,7 +933,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -612,7 +968,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -823,50 +1179,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.26953125" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" customWidth="1"/>
-    <col min="14" max="14" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B1" s="25">
-        <v>2</v>
-      </c>
-      <c r="J1" s="25">
+    <row r="1" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B1" s="19">
+        <v>2</v>
+      </c>
+      <c r="J1" s="19">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+    <row r="2" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="J2" s="21" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="J2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="23"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -892,7 +1248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B4" s="9">
         <v>1</v>
       </c>
@@ -918,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B5" s="9">
         <v>2</v>
       </c>
@@ -944,8 +1300,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B6" s="25">
+    <row r="6" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B6" s="19">
         <v>5</v>
       </c>
       <c r="J6" s="3">
@@ -958,16 +1314,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
+    <row r="7" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
@@ -983,11 +1339,11 @@
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B9" s="12">
         <v>1</v>
       </c>
@@ -1003,14 +1359,14 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="23"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24"/>
+    </row>
+    <row r="10" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B10" s="12">
         <v>2</v>
       </c>
@@ -1039,7 +1395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="J11" s="4">
         <v>1</v>
       </c>
@@ -1053,8 +1409,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B12" s="25">
+    <row r="12" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B12" s="19">
         <v>7</v>
       </c>
       <c r="J12" s="4">
@@ -1070,16 +1426,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B13" s="24" t="s">
+    <row r="13" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B13" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
       <c r="J13" s="3">
         <v>3</v>
       </c>
@@ -1093,7 +1449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
@@ -1116,7 +1472,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B15" s="14">
         <v>1</v>
       </c>
@@ -1136,11 +1492,11 @@
       <c r="H15" s="11">
         <v>43713</v>
       </c>
-      <c r="J15" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="J15" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
         <v>2</v>
       </c>
@@ -1160,14 +1516,14 @@
       <c r="H16" s="11">
         <v>43713</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="23"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="24"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1181,15 +1537,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B18" s="24" t="s">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
       <c r="J18" s="5">
         <v>1</v>
       </c>
@@ -1203,7 +1559,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
@@ -1235,7 +1591,7 @@
         <v>44256</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>1</v>
       </c>
@@ -1254,11 +1610,11 @@
       <c r="G20" s="5">
         <v>1</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="19">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>2</v>
       </c>
@@ -1277,14 +1633,14 @@
       <c r="G21" s="5">
         <v>1</v>
       </c>
-      <c r="J21" s="21" t="s">
+      <c r="J21" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="23"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="24"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <v>3</v>
       </c>
@@ -1316,7 +1672,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J23" s="8">
         <v>1</v>
       </c>
@@ -1330,7 +1686,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J24" s="8">
         <v>2</v>
       </c>
@@ -1344,16 +1700,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B25" s="24" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1370,7 +1726,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="13">
         <v>1</v>
       </c>
@@ -1387,7 +1743,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>2</v>
       </c>
@@ -1404,7 +1760,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <v>3</v>
       </c>
@@ -1421,18 +1777,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B32" s="24" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>66</v>
       </c>
@@ -1455,7 +1811,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>1</v>
       </c>
@@ -1476,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>2</v>
       </c>
@@ -1497,23 +1853,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B37" s="25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="19">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B38" s="19" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>73</v>
       </c>
@@ -1536,7 +1892,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>1</v>
       </c>
@@ -1559,7 +1915,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>2</v>
       </c>
@@ -1582,26 +1938,26 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B43" s="25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="19">
         <v>9</v>
       </c>
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B44" s="21" t="s">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="24"/>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>85</v>
       </c>
@@ -1618,7 +1974,7 @@
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>1</v>
       </c>
@@ -1635,7 +1991,7 @@
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="3">
         <v>2</v>
       </c>
@@ -1674,13 +2030,1227 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:Y57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M56" sqref="K56:M57"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" customWidth="1"/>
+    <col min="22" max="22" width="5" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="K9" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="11">
+        <f ca="1">TODAY()</f>
+        <v>43747</v>
+      </c>
+      <c r="F11" s="11">
+        <f ca="1">TODAY()</f>
+        <v>43747</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K11" s="32">
+        <v>1</v>
+      </c>
+      <c r="L11" s="33">
+        <v>1</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="N11" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="O11" s="30"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="11">
+        <f ca="1">TODAY()</f>
+        <v>43747</v>
+      </c>
+      <c r="F12" s="11">
+        <f ca="1">TODAY()</f>
+        <v>43747</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K12" s="32">
+        <v>2</v>
+      </c>
+      <c r="L12" s="33">
+        <v>2</v>
+      </c>
+      <c r="M12" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="N12" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="O12" s="30"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="K15" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="L15" s="25"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="39">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="32">
+        <v>1</v>
+      </c>
+      <c r="E17" s="36">
+        <v>1</v>
+      </c>
+      <c r="F17" s="11">
+        <f ca="1">TODAY()</f>
+        <v>43747</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="33">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="M17" s="29"/>
+      <c r="N17" s="31"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="39">
+        <v>2</v>
+      </c>
+      <c r="C18" s="9">
+        <v>2</v>
+      </c>
+      <c r="D18" s="32">
+        <v>1</v>
+      </c>
+      <c r="E18" s="36">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11">
+        <f ca="1">TODAY()</f>
+        <v>43747</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="33">
+        <v>2</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" s="29"/>
+      <c r="N18" s="31"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K19" s="33">
+        <v>3</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="K22" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="L22" s="25"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="35">
+        <v>1</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="16">
+        <v>1</v>
+      </c>
+      <c r="E23" s="27">
+        <v>3</v>
+      </c>
+      <c r="F23" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="K23" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="35">
+        <v>2</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="16">
+        <v>1</v>
+      </c>
+      <c r="E24" s="27">
+        <v>3</v>
+      </c>
+      <c r="F24" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="K24" s="33">
+        <v>1</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K25" s="33">
+        <v>2</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="K26" s="33">
+        <v>3</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="16">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16">
+        <v>1</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="30"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="16">
+        <v>2</v>
+      </c>
+      <c r="C29" s="9">
+        <v>2</v>
+      </c>
+      <c r="D29" s="16">
+        <v>1</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K30" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="24"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="K32" s="16">
+        <v>1</v>
+      </c>
+      <c r="L32" s="35">
+        <v>1</v>
+      </c>
+      <c r="M32" s="38">
+        <v>1</v>
+      </c>
+      <c r="N32" s="27">
+        <v>4000</v>
+      </c>
+      <c r="O32" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="P32" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>1</v>
+      </c>
+      <c r="R32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="K33" s="16">
+        <v>2</v>
+      </c>
+      <c r="L33" s="35">
+        <v>2</v>
+      </c>
+      <c r="M33" s="38">
+        <v>1</v>
+      </c>
+      <c r="N33" s="27">
+        <v>10000</v>
+      </c>
+      <c r="O33" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="P33" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>1</v>
+      </c>
+      <c r="R33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B34" s="16">
+        <v>1</v>
+      </c>
+      <c r="C34" s="39">
+        <v>1</v>
+      </c>
+      <c r="D34" s="17">
+        <v>43505</v>
+      </c>
+      <c r="E34" s="17">
+        <v>43505</v>
+      </c>
+      <c r="F34" s="27">
+        <v>1</v>
+      </c>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="16">
+        <v>2</v>
+      </c>
+      <c r="C35" s="39">
+        <v>2</v>
+      </c>
+      <c r="D35" s="17">
+        <v>43505</v>
+      </c>
+      <c r="E35" s="17">
+        <v>43505</v>
+      </c>
+      <c r="F35" s="27">
+        <v>0</v>
+      </c>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="J35" s="25"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="I36" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="15"/>
+      <c r="I37" s="40">
+        <v>1</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K37" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="29"/>
+      <c r="I38" s="40">
+        <v>2</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q38" s="29"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B39" s="16">
+        <v>1</v>
+      </c>
+      <c r="C39" s="9">
+        <v>1</v>
+      </c>
+      <c r="D39" s="41">
+        <v>1</v>
+      </c>
+      <c r="E39" s="17">
+        <v>43505</v>
+      </c>
+      <c r="F39" s="31"/>
+      <c r="I39" s="40">
+        <v>3</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K39" s="38">
+        <v>1</v>
+      </c>
+      <c r="L39" s="13">
+        <v>1</v>
+      </c>
+      <c r="M39" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="N39" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="O39" s="3">
+        <v>1</v>
+      </c>
+      <c r="P39" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="29"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B40" s="16">
+        <v>2</v>
+      </c>
+      <c r="C40" s="9">
+        <v>2</v>
+      </c>
+      <c r="D40" s="41">
+        <v>1</v>
+      </c>
+      <c r="E40" s="17">
+        <v>43505</v>
+      </c>
+      <c r="F40" s="31"/>
+      <c r="K40" s="38">
+        <v>2</v>
+      </c>
+      <c r="L40" s="13">
+        <v>1</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="N40" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="O40" s="3">
+        <v>1</v>
+      </c>
+      <c r="P40" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="29"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B43" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="15"/>
+      <c r="K43" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="24"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H44" s="29"/>
+      <c r="K44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="16">
+        <v>1</v>
+      </c>
+      <c r="C45" s="39">
+        <v>1</v>
+      </c>
+      <c r="D45" s="38">
+        <v>1</v>
+      </c>
+      <c r="E45" s="28">
+        <v>5000</v>
+      </c>
+      <c r="F45" s="27">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="29"/>
+      <c r="K45" s="13">
+        <v>1</v>
+      </c>
+      <c r="L45" s="37">
+        <v>1</v>
+      </c>
+      <c r="M45" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="N45" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="O45" s="3">
+        <v>1</v>
+      </c>
+      <c r="P45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B46" s="16">
+        <v>2</v>
+      </c>
+      <c r="C46" s="39">
+        <v>2</v>
+      </c>
+      <c r="D46" s="38">
+        <v>2</v>
+      </c>
+      <c r="E46" s="28">
+        <v>10000</v>
+      </c>
+      <c r="F46" s="27">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="29"/>
+      <c r="K46" s="13">
+        <v>2</v>
+      </c>
+      <c r="L46" s="37">
+        <v>1</v>
+      </c>
+      <c r="M46" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="N46" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="O46" s="3">
+        <v>1</v>
+      </c>
+      <c r="P46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K48" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="L48" s="23"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="23"/>
+      <c r="P48" s="24"/>
+    </row>
+    <row r="49" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K49" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K50" s="37">
+        <v>1</v>
+      </c>
+      <c r="L50" s="8">
+        <v>1</v>
+      </c>
+      <c r="M50" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="N50" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="O50" s="3">
+        <v>1</v>
+      </c>
+      <c r="P50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K51" s="37">
+        <v>2</v>
+      </c>
+      <c r="L51" s="8">
+        <v>1</v>
+      </c>
+      <c r="M51" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="N51" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="O51" s="3">
+        <v>1</v>
+      </c>
+      <c r="P51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K54" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="L54" s="23"/>
+      <c r="M54" s="23"/>
+      <c r="N54" s="23"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="15"/>
+    </row>
+    <row r="55" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K55" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="P55" s="29"/>
+    </row>
+    <row r="56" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K56" s="8">
+        <v>1</v>
+      </c>
+      <c r="L56" s="16">
+        <v>1</v>
+      </c>
+      <c r="M56" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="N56" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="O56" s="3">
+        <v>1</v>
+      </c>
+      <c r="P56" s="29"/>
+    </row>
+    <row r="57" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K57" s="8">
+        <v>2</v>
+      </c>
+      <c r="L57" s="16">
+        <v>1</v>
+      </c>
+      <c r="M57" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="N57" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="O57" s="3">
+        <v>1</v>
+      </c>
+      <c r="P57" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="K48:P48"/>
+    <mergeCell ref="K54:O54"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="K30:R30"/>
+    <mergeCell ref="K37:P37"/>
+    <mergeCell ref="K43:P43"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="B2:W2"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="K9:N9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1690,7 +3260,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
all the latest changes are not committed
</commit_message>
<xml_diff>
--- a/application-service/src/test/resources/document/ExaminationModule_Schema.xlsx
+++ b/application-service/src/test/resources/document/ExaminationModule_Schema.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="193">
   <si>
     <t>Exam</t>
   </si>
@@ -597,6 +597,9 @@
   </si>
   <si>
     <t>delete</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -878,6 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -896,7 +900,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1203,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,21 +1235,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B2" s="41" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="J2" s="38" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="J2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
-    </row>
-    <row r="3" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1271,8 +1274,11 @@
       <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="M3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="9">
         <v>1</v>
       </c>
@@ -1297,8 +1303,11 @@
       <c r="L4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="9">
         <v>2</v>
       </c>
@@ -1323,8 +1332,11 @@
       <c r="L5" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="M5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="19">
         <v>5</v>
       </c>
@@ -1337,17 +1349,20 @@
       <c r="L6" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B7" s="41" t="s">
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-    </row>
-    <row r="8" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
@@ -1367,7 +1382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <v>1</v>
       </c>
@@ -1383,14 +1398,14 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="40"/>
-    </row>
-    <row r="10" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
         <v>2</v>
       </c>
@@ -1419,7 +1434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J11" s="4">
         <v>1</v>
       </c>
@@ -1433,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="19">
         <v>7</v>
       </c>
@@ -1450,16 +1465,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B13" s="41" t="s">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
       <c r="J13" s="3">
         <v>3</v>
       </c>
@@ -1473,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
@@ -1496,7 +1511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="14">
         <v>1</v>
       </c>
@@ -1540,12 +1555,12 @@
       <c r="H16" s="11">
         <v>43713</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="J16" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="41"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J17" s="1" t="s">
@@ -1560,25 +1575,25 @@
       <c r="M17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N17" s="42" t="s">
+      <c r="N17" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="O17" s="42" t="s">
+      <c r="O17" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="P17" s="42" t="s">
+      <c r="P17" s="36" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
       <c r="J18" s="5">
         <v>1</v>
       </c>
@@ -1666,12 +1681,12 @@
       <c r="G21" s="5">
         <v>1</v>
       </c>
-      <c r="J21" s="38" t="s">
+      <c r="J21" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="41"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
@@ -1704,6 +1719,12 @@
       <c r="M22" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="N22" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="O22" s="36" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J23" s="8">
@@ -1734,13 +1755,13 @@
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
@@ -1811,15 +1832,15 @@
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
@@ -1892,15 +1913,15 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
@@ -1980,12 +2001,12 @@
       <c r="H43" s="18"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="38" t="s">
+      <c r="B44" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="41"/>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
@@ -2098,30 +2119,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
       <c r="X2" s="15"/>
       <c r="Y2" s="15"/>
     </row>
@@ -2280,20 +2301,20 @@
       <c r="W5" s="3"/>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="K9" s="41" t="s">
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="K9" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
       <c r="Q9" s="15"/>
@@ -2345,11 +2366,11 @@
       </c>
       <c r="E11" s="11">
         <f ca="1">TODAY()</f>
-        <v>43755</v>
+        <v>43764</v>
       </c>
       <c r="F11" s="11">
         <f ca="1">TODAY()</f>
-        <v>43755</v>
+        <v>43764</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>122</v>
@@ -2382,11 +2403,11 @@
       </c>
       <c r="E12" s="11">
         <f ca="1">TODAY()</f>
-        <v>43755</v>
+        <v>43764</v>
       </c>
       <c r="F12" s="11">
         <f ca="1">TODAY()</f>
-        <v>43755</v>
+        <v>43764</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>122</v>
@@ -2408,19 +2429,19 @@
       <c r="Q12" s="23"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="K15" s="41" t="s">
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="K15" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="L15" s="41"/>
+      <c r="L15" s="42"/>
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
     </row>
@@ -2470,7 +2491,7 @@
       </c>
       <c r="F17" s="11">
         <f ca="1">TODAY()</f>
-        <v>43755</v>
+        <v>43764</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
@@ -2502,7 +2523,7 @@
       </c>
       <c r="F18" s="11">
         <f ca="1">TODAY()</f>
-        <v>43755</v>
+        <v>43764</v>
       </c>
       <c r="G18" s="3">
         <v>1</v>
@@ -2528,13 +2549,13 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
     </row>
@@ -2556,10 +2577,10 @@
       </c>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
-      <c r="K22" s="41" t="s">
+      <c r="K22" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="L22" s="41"/>
+      <c r="L22" s="42"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="29">
@@ -2620,12 +2641,12 @@
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -2688,16 +2709,16 @@
       <c r="H29" s="23"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K30" s="38" t="s">
+      <c r="K30" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
-      <c r="R30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="41"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K31" s="1" t="s">
@@ -2726,13 +2747,13 @@
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="K32" s="16">
@@ -2840,10 +2861,10 @@
       </c>
       <c r="G35" s="23"/>
       <c r="H35" s="23"/>
-      <c r="I35" s="41" t="s">
+      <c r="I35" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="J35" s="41"/>
+      <c r="J35" s="42"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I36" s="1" t="s">
@@ -2854,12 +2875,12 @@
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
       <c r="F37" s="15"/>
       <c r="I37" s="34">
         <v>1</v>
@@ -2867,14 +2888,14 @@
       <c r="J37" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="K37" s="38" t="s">
+      <c r="K37" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="L37" s="39"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="39"/>
-      <c r="O37" s="39"/>
-      <c r="P37" s="40"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="40"/>
+      <c r="N37" s="40"/>
+      <c r="O37" s="40"/>
+      <c r="P37" s="41"/>
       <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
     </row>
@@ -2993,23 +3014,23 @@
       <c r="Q40" s="23"/>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
       <c r="H43" s="15"/>
-      <c r="K43" s="38" t="s">
+      <c r="K43" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
-      <c r="O43" s="39"/>
-      <c r="P43" s="40"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="40"/>
+      <c r="N43" s="40"/>
+      <c r="O43" s="40"/>
+      <c r="P43" s="41"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
@@ -3129,14 +3150,14 @@
       </c>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K48" s="38" t="s">
+      <c r="K48" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="L48" s="39"/>
-      <c r="M48" s="39"/>
-      <c r="N48" s="39"/>
-      <c r="O48" s="39"/>
-      <c r="P48" s="40"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="40"/>
+      <c r="N48" s="40"/>
+      <c r="O48" s="40"/>
+      <c r="P48" s="41"/>
     </row>
     <row r="49" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K49" s="1" t="s">
@@ -3199,13 +3220,13 @@
       </c>
     </row>
     <row r="54" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K54" s="38" t="s">
+      <c r="K54" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="L54" s="39"/>
-      <c r="M54" s="39"/>
-      <c r="N54" s="39"/>
-      <c r="O54" s="40"/>
+      <c r="L54" s="40"/>
+      <c r="M54" s="40"/>
+      <c r="N54" s="40"/>
+      <c r="O54" s="41"/>
       <c r="P54" s="15"/>
     </row>
     <row r="55" spans="11:16" x14ac:dyDescent="0.25">
@@ -3264,6 +3285,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="B2:W2"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="K9:N9"/>
     <mergeCell ref="K48:P48"/>
     <mergeCell ref="K54:O54"/>
     <mergeCell ref="I35:J35"/>
@@ -3273,14 +3302,6 @@
     <mergeCell ref="K43:P43"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="B2:W2"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="B26:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>